<commit_message>
add the missing extra header row
</commit_message>
<xml_diff>
--- a/tests/modules/local/create_batch_tsvs/test_genbank.xlsx
+++ b/tests/modules/local/create_batch_tsvs/test_genbank.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjd0\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\02.scratch\tostadas-staging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{969794AB-10BC-4EEE-BB36-104B532355AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206A70CA-522B-4952-BA2E-2053475D190B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="14400" windowHeight="7270" xr2:uid="{03E92ED3-FA45-4C94-9E80-BAE2B9F8AD48}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{03E92ED3-FA45-4C94-9E80-BAE2B9F8AD48}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="86">
   <si>
     <t>sample_name</t>
   </si>
@@ -146,9 +146,6 @@
     <t>gff_path</t>
   </si>
   <si>
-    <t>ncbi_sequence_name_sra</t>
-  </si>
-  <si>
     <t>illumina_sequencing_instrument</t>
   </si>
   <si>
@@ -291,6 +288,12 @@
   </si>
   <si>
     <t>NM_012345</t>
+  </si>
+  <si>
+    <t>ncbi-spuid-sra</t>
+  </si>
+  <si>
+    <t>NCBI Submission Info</t>
   </si>
 </sst>
 </file>
@@ -699,312 +702,317 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA30646F-759E-42ED-A545-C7B21EDA3D0D}">
-  <dimension ref="A1:BE2"/>
+  <dimension ref="A1:BE3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:57" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="BE1" s="1" t="s">
-        <v>56</v>
+      <c r="A1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:57" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AS2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AV2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AW2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AX2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AZ2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BA2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BB2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BC2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BD2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BE2" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:57" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="2">
+        <v>123456</v>
+      </c>
+      <c r="C3" s="2">
+        <v>654321</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="2">
-        <v>123456</v>
-      </c>
-      <c r="C2" s="2">
-        <v>654321</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="F3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q2" s="2" t="s">
+      <c r="S3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="T3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="S2" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="W3" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="Y3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="X2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2" t="s">
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
-      <c r="AE2" s="2"/>
-      <c r="AF2" s="2" t="s">
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="AG2" s="2"/>
-      <c r="AH2" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AJ2" s="2"/>
-      <c r="AK2" s="2" t="s">
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AM3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AM2" s="2" t="s">
+      <c r="AN3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AN2" s="2" t="s">
+      <c r="AO3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AO2" s="2" t="s">
+      <c r="AP3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="AP2" s="2" t="s">
+      <c r="AQ3" s="2"/>
+      <c r="AR3" s="2"/>
+      <c r="AS3" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AQ2" s="2"/>
-      <c r="AR2" s="2"/>
-      <c r="AS2" s="2" t="s">
+      <c r="AT3" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AT2" s="2" t="s">
+      <c r="AU3" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AU2" s="2" t="s">
+      <c r="AV3" s="2"/>
+      <c r="AW3" s="2"/>
+      <c r="AX3" s="2"/>
+      <c r="AY3" s="2"/>
+      <c r="AZ3" s="2"/>
+      <c r="BA3" s="2"/>
+      <c r="BB3" s="2"/>
+      <c r="BC3" s="2"/>
+      <c r="BD3" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="AV2" s="2"/>
-      <c r="AW2" s="2"/>
-      <c r="AX2" s="2"/>
-      <c r="AY2" s="2"/>
-      <c r="AZ2" s="2"/>
-      <c r="BA2" s="2"/>
-      <c r="BB2" s="2"/>
-      <c r="BC2" s="2"/>
-      <c r="BD2" s="2" t="s">
+      <c r="BE3" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="BE2" s="2" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>